<commit_message>
Updated feedback loop to send all local data to server
</commit_message>
<xml_diff>
--- a/Global protocol.xlsx
+++ b/Global protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loure\Dropbox\Lourenço\Faculdade\5A1S\SCDTR\SCDTR-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E48AADE-71A9-401A-8952-16592664E102}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22CD2AB-6C62-4AD3-B225-54C709D086D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
   <si>
     <t>Command</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>l &lt;i&gt; &lt;val&gt;</t>
-  </si>
-  <si>
-    <t>EM FALTA</t>
   </si>
   <si>
     <t>Get current duty cycle
@@ -172,10 +169,6 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;i&gt; &lt;val&gt;</t>
-  </si>
-  <si>
-    <t>&lt;val&gt; is floating point number expressing
-illuminance control reference in lux.</t>
   </si>
   <si>
     <t>Get instantaneous
@@ -430,6 +423,36 @@
   </si>
   <si>
     <t>&lt;val&gt; is a Boolean flag: 1 - ready to begin negotiation  0 - not negotiating</t>
+  </si>
+  <si>
+    <t>Arduino Function</t>
+  </si>
+  <si>
+    <t>sendLuxReading(&lt;val&gt;)</t>
+  </si>
+  <si>
+    <t>sendPwm(&lt;val&gt;)</t>
+  </si>
+  <si>
+    <t>sendOccupancy(&lt;val&gt;)</t>
+  </si>
+  <si>
+    <t>sendLuxLowerBound(&lt;v&gt;)</t>
+  </si>
+  <si>
+    <t>sendLuxBackground(&lt;v&gt;)</t>
+  </si>
+  <si>
+    <t>sendLuxRef(&lt;v&gt;)</t>
+  </si>
+  <si>
+    <t>sendNegotiationState(&lt;v&gt;)</t>
+  </si>
+  <si>
+    <t>sendNegotiation(&lt;v1&gt;,&lt;v2&gt;)</t>
+  </si>
+  <si>
+    <t>&lt;val&gt; is floating point number expressing the illuminance PWM control reference (obtained by consensus) between 0 and 5.</t>
   </si>
 </sst>
 </file>
@@ -964,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -978,13 +1001,14 @@
     <col min="4" max="4" width="22.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="43.58203125" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.58203125" customWidth="1"/>
-    <col min="9" max="9" width="9.58203125" customWidth="1"/>
-    <col min="10" max="1025" width="8.58203125" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.58203125" customWidth="1"/>
+    <col min="10" max="10" width="9.58203125" customWidth="1"/>
+    <col min="11" max="1026" width="8.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1004,10 +1028,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="42" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1018,352 +1045,387 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E2" s="1">
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="1">
+        <v>80</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="1">
         <v>2</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="28" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="28" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1">
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="1">
+        <v>79</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" s="6">
         <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="42" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5" s="6">
         <v>4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="7">
+        <v>84</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" s="6">
         <v>4</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="7">
+        <v>85</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" s="6">
         <v>4</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="7">
+        <v>99</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="1">
+        <v>82</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="28" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="1">
+        <v>89</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="42" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" ht="42" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="42" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="28" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="56" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="56" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="F13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" ht="56" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="56" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="F14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="56" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="56" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="42" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="42" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="56" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="56" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="F17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="42" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="42" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="F18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="F19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="37.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:7" ht="56" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="37.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:6" ht="56" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="C21" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="F21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="84" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="84" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="C22" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="F22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="56" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="B23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="56" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="G23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>

</xml_diff>

<commit_message>
changed sendLuxRef to sendPWMRef
</commit_message>
<xml_diff>
--- a/Global protocol.xlsx
+++ b/Global protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loure\Dropbox\Lourenço\Faculdade\5A1S\SCDTR\SCDTR-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22CD2AB-6C62-4AD3-B225-54C709D086D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50880F80-BB96-4248-99BF-3FB69FCB6948}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,9 +443,6 @@
     <t>sendLuxBackground(&lt;v&gt;)</t>
   </si>
   <si>
-    <t>sendLuxRef(&lt;v&gt;)</t>
-  </si>
-  <si>
     <t>sendNegotiationState(&lt;v&gt;)</t>
   </si>
   <si>
@@ -453,6 +450,9 @@
   </si>
   <si>
     <t>&lt;val&gt; is floating point number expressing the illuminance PWM control reference (obtained by consensus) between 0 and 5.</t>
+  </si>
+  <si>
+    <t>sendPWMRef(&lt;v&gt;)</t>
   </si>
 </sst>
 </file>
@@ -990,7 +990,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1182,10 +1182,10 @@
         <v>4</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="H7" s="7">
         <v>2</v>
@@ -1205,7 +1205,7 @@
         <v>82</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
@@ -1225,7 +1225,7 @@
         <v>89</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>

</xml_diff>